<commit_message>
licor data and coding
</commit_message>
<xml_diff>
--- a/Trait_Data.xlsx
+++ b/Trait_Data.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fernbromley/Desktop/AVCA_BANWR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9753F365-3F83-234A-9E6D-A38D018438D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32F6FD70-D0BF-904A-B46A-578810D7C556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="28720" windowHeight="17180" xr2:uid="{4A808A7B-9666-F048-9C16-1E6E06F0F3E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$F$1</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$F$2:$F$81</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!#REF!</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!#REF!</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -42,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="16">
   <si>
     <t>Species</t>
   </si>
@@ -72,6 +66,24 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>Dry_weight_plus_coinbag_g</t>
+  </si>
+  <si>
+    <t>Bag_g</t>
+  </si>
+  <si>
+    <t>Area_mm2</t>
+  </si>
+  <si>
+    <t>Dry_weight_mg</t>
+  </si>
+  <si>
+    <t>SLA_mm2_mg</t>
+  </si>
+  <si>
+    <t>LWC_mgmg</t>
   </si>
 </sst>
 </file>
@@ -451,20 +463,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED2590CA-9E92-344E-9414-AAC64875E186}">
-  <dimension ref="A1:E81"/>
+  <dimension ref="A1:K81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E52" sqref="E52"/>
+    <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -478,10 +494,28 @@
         <v>7</v>
       </c>
       <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -494,8 +528,34 @@
       <c r="D2">
         <v>9.0950000000000003E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E2">
+        <v>1.2295400000000001</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G2">
+        <f>E2-F2</f>
+        <v>4.5341538461538544E-2</v>
+      </c>
+      <c r="H2">
+        <f>C2*100</f>
+        <v>516.5</v>
+      </c>
+      <c r="I2">
+        <f>G2*1000</f>
+        <v>45.341538461538548</v>
+      </c>
+      <c r="J2">
+        <f>H2/I2</f>
+        <v>11.391320575461434</v>
+      </c>
+      <c r="K2">
+        <f>(D2-G2)/D2</f>
+        <v>0.50146741658561256</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -508,8 +568,34 @@
       <c r="D3">
         <v>7.6689999999999994E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E3">
+        <v>1.23783</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G66" si="0">E3-F3</f>
+        <v>5.3631538461538453E-2</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H66" si="1">C3*100</f>
+        <v>434.99999999999994</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I66" si="2">G3*1000</f>
+        <v>53.631538461538454</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J66" si="3">H3/I3</f>
+        <v>8.110899155204315</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K66" si="4">(D3-G3)/D3</f>
+        <v>0.30067103323068906</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -522,8 +608,34 @@
       <c r="D4">
         <v>7.3709999999999998E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E4">
+        <v>1.2053199999999999</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>2.1121538461538414E-2</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="1"/>
+        <v>405.79999999999995</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="2"/>
+        <v>21.121538461538414</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="3"/>
+        <v>19.212615631145791</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="4"/>
+        <v>0.7134508416559705</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -536,8 +648,34 @@
       <c r="D5">
         <v>4.9950000000000001E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E5">
+        <v>1.2261500000000001</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>4.195153846153854E-2</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>225.2</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="2"/>
+        <v>41.95153846153854</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="3"/>
+        <v>5.3680987219685612</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="4"/>
+        <v>0.16012936012935858</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -550,8 +688,34 @@
       <c r="D6">
         <v>0.11035</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E6">
+        <v>1.2351399999999999</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>5.0941538461538372E-2</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>454</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="2"/>
+        <v>50.941538461538372</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="3"/>
+        <v>8.9121768543126514</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="4"/>
+        <v>0.53836394688229838</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -564,8 +728,34 @@
       <c r="D7">
         <v>8.5139999999999993E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E7">
+        <v>1.2345600000000001</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>5.0361538461538569E-2</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>483.4</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>50.361538461538572</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="3"/>
+        <v>9.5985947762333677</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="4"/>
+        <v>0.40848557127626767</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -578,8 +768,34 @@
       <c r="D8">
         <v>6.8040000000000003E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E8">
+        <v>1.21584</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>3.1641538461538499E-2</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>330.1</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="2"/>
+        <v>31.641538461538499</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="3"/>
+        <v>10.432488938590936</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="4"/>
+        <v>0.53495681273458995</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -592,8 +808,34 @@
       <c r="D9">
         <v>0.10335999999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E9">
+        <v>1.26759</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>8.3391538461538461E-2</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>484.1</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="2"/>
+        <v>83.39153846153846</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="3"/>
+        <v>5.8051453292623307</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="4"/>
+        <v>0.19319331983805663</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -606,8 +848,34 @@
       <c r="D10">
         <v>8.0990000000000006E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E10">
+        <v>1.1841600000000001</v>
+      </c>
+      <c r="F10">
+        <v>1.16543</v>
+      </c>
+      <c r="G10">
+        <f>E10-F10</f>
+        <v>1.8730000000000135E-2</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>309.90000000000003</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="2"/>
+        <v>18.730000000000135</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="3"/>
+        <v>16.545648691937949</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="4"/>
+        <v>0.76873688109643001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -620,8 +888,34 @@
       <c r="D11">
         <v>9.2509999999999995E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E11">
+        <v>1.22529</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>4.1091538461538457E-2</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>525</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="2"/>
+        <v>41.091538461538455</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="3"/>
+        <v>12.776352983021024</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="4"/>
+        <v>0.55581517174858441</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -634,8 +928,34 @@
       <c r="D12">
         <v>3.78E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E12">
+        <v>1.1842999999999999</v>
+      </c>
+      <c r="F12">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>1.015384615383752E-4</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>179.5</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="2"/>
+        <v>0.1015384615383752</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="3"/>
+        <v>1767.8030303045334</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="4"/>
+        <v>0.99731379731379954</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -648,8 +968,34 @@
       <c r="D13">
         <v>7.1129999999999999E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E13">
+        <v>1.25213</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>6.7931538461538432E-2</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>409.6</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="2"/>
+        <v>67.931538461538437</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="3"/>
+        <v>6.0295999365877435</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="4"/>
+        <v>4.4966421178990114E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -662,8 +1008,34 @@
       <c r="D14">
         <v>9.2340000000000005E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E14">
+        <v>1.22715</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>4.295153846153843E-2</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>443.70000000000005</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="2"/>
+        <v>42.951538461538433</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="3"/>
+        <v>10.330246968855784</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="4"/>
+        <v>0.53485446760300603</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -676,8 +1048,34 @@
       <c r="D15">
         <v>6.7830000000000001E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E15">
+        <v>1.2301599999999999</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>4.5961538461538387E-2</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>385.1</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="2"/>
+        <v>45.961538461538389</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="3"/>
+        <v>8.3787447698744906</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="4"/>
+        <v>0.32240102518740399</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -690,8 +1088,34 @@
       <c r="D16">
         <v>7.9130000000000006E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16">
+        <v>1.24363</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>5.943153846153848E-2</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="1"/>
+        <v>337.1</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="2"/>
+        <v>59.43153846153848</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="3"/>
+        <v>5.672072585133507</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="4"/>
+        <v>0.24893796965072065</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -704,8 +1128,34 @@
       <c r="D17">
         <v>9.9669999999999995E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17">
+        <v>1.2333499999999999</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>4.9151538461538413E-2</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="1"/>
+        <v>600</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="2"/>
+        <v>49.151538461538415</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="3"/>
+        <v>12.207145875393223</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="4"/>
+        <v>0.50685724429077539</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -718,8 +1168,34 @@
       <c r="D18">
         <v>4.0189999999999997E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18">
+        <v>1.1802900000000001</v>
+      </c>
+      <c r="F18">
+        <v>1.1794800000000001</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>8.099999999999774E-4</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="1"/>
+        <v>194</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="2"/>
+        <v>0.8099999999999774</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="3"/>
+        <v>239.50617283951286</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="4"/>
+        <v>0.97984573276934617</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -732,8 +1208,34 @@
       <c r="D19">
         <v>7.0480000000000001E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19">
+        <v>1.2085999999999999</v>
+      </c>
+      <c r="F19" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>2.4401538461538363E-2</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="1"/>
+        <v>444.4</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="2"/>
+        <v>24.401538461538365</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="3"/>
+        <v>18.21196645860924</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="4"/>
+        <v>0.65378066882039776</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -746,8 +1248,34 @@
       <c r="D20">
         <v>0.10133</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20">
+        <v>1.22204</v>
+      </c>
+      <c r="F20" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="0"/>
+        <v>3.7841538461538482E-2</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="1"/>
+        <v>572.29999999999995</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="2"/>
+        <v>37.841538461538484</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="3"/>
+        <v>15.123592308005032</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="4"/>
+        <v>0.6265514806914193</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -760,8 +1288,34 @@
       <c r="D21">
         <v>0.10014000000000001</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21">
+        <v>1.23613</v>
+      </c>
+      <c r="F21" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>5.1931538461538418E-2</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="1"/>
+        <v>501.1</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="2"/>
+        <v>51.931538461538416</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="3"/>
+        <v>9.6492423456918228</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="4"/>
+        <v>0.48141064048793275</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -774,8 +1328,34 @@
       <c r="D22">
         <v>0.1079</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22">
+        <v>1.22506</v>
+      </c>
+      <c r="F22" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="0"/>
+        <v>4.0861538461538505E-2</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="1"/>
+        <v>569.80000000000007</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="2"/>
+        <v>40.861538461538501</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="3"/>
+        <v>13.94465361445782</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="4"/>
+        <v>0.62130177514792861</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -788,8 +1368,34 @@
       <c r="D23">
         <v>0.14849000000000001</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E23">
+        <v>1.21122</v>
+      </c>
+      <c r="F23" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="0"/>
+        <v>2.702153846153843E-2</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="1"/>
+        <v>909</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="2"/>
+        <v>27.02153846153843</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="3"/>
+        <v>33.639831473468497</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="4"/>
+        <v>0.81802452379595647</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -802,8 +1408,34 @@
       <c r="D24">
         <v>9.4439999999999996E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E24">
+        <v>1.2391399999999999</v>
+      </c>
+      <c r="F24" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="0"/>
+        <v>5.4941538461538375E-2</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="1"/>
+        <v>648.80000000000007</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="2"/>
+        <v>54.941538461538372</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="3"/>
+        <v>11.808915770609339</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="4"/>
+        <v>0.41823868634542166</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>5</v>
       </c>
@@ -816,8 +1448,34 @@
       <c r="D25">
         <v>0.1061</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E25">
+        <v>1.2048700000000001</v>
+      </c>
+      <c r="F25" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="0"/>
+        <v>2.0671538461538574E-2</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="1"/>
+        <v>617.79999999999995</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="2"/>
+        <v>20.671538461538574</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="3"/>
+        <v>29.886503181631955</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="4"/>
+        <v>0.80516928876966476</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>5</v>
       </c>
@@ -830,8 +1488,34 @@
       <c r="D26">
         <v>6.583E-2</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E26">
+        <v>1.2099299999999999</v>
+      </c>
+      <c r="F26" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="0"/>
+        <v>2.5731538461538417E-2</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="1"/>
+        <v>434.3</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="2"/>
+        <v>25.731538461538417</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="3"/>
+        <v>16.878120235568474</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="4"/>
+        <v>0.60912139660430786</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -844,8 +1528,34 @@
       <c r="D27">
         <v>7.9420000000000004E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E27">
+        <v>1.20529</v>
+      </c>
+      <c r="F27" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="0"/>
+        <v>2.1091538461538439E-2</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="1"/>
+        <v>474.5</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="2"/>
+        <v>21.091538461538441</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="3"/>
+        <v>22.497173492833458</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="4"/>
+        <v>0.73443038955504358</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>5</v>
       </c>
@@ -858,8 +1568,34 @@
       <c r="D28">
         <v>6.13E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E28">
+        <v>1.2113499999999999</v>
+      </c>
+      <c r="F28" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="0"/>
+        <v>2.7151538461538394E-2</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="1"/>
+        <v>287.59999999999997</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="2"/>
+        <v>27.151538461538394</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="3"/>
+        <v>10.592401620534348</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="4"/>
+        <v>0.55707115070899849</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>5</v>
       </c>
@@ -872,8 +1608,34 @@
       <c r="D29">
         <v>5.4480000000000001E-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E29">
+        <v>1.20472</v>
+      </c>
+      <c r="F29" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="0"/>
+        <v>2.052153846153848E-2</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="1"/>
+        <v>291.10000000000002</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="2"/>
+        <v>20.52153846153848</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="3"/>
+        <v>14.185096334058013</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="4"/>
+        <v>0.62331977860612187</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>5</v>
       </c>
@@ -886,8 +1648,34 @@
       <c r="D30">
         <v>4.1439999999999998E-2</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E30">
+        <v>1.19286</v>
+      </c>
+      <c r="F30" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="0"/>
+        <v>8.6615384615384983E-3</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="1"/>
+        <v>263.89999999999998</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="2"/>
+        <v>8.6615384615384983</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="3"/>
+        <v>30.468028419182815</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="4"/>
+        <v>0.79098604098604008</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>5</v>
       </c>
@@ -900,8 +1688,34 @@
       <c r="D31">
         <v>8.4680000000000005E-2</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E31">
+        <v>1.2072499999999999</v>
+      </c>
+      <c r="F31" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="0"/>
+        <v>2.3051538461538401E-2</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="1"/>
+        <v>538.69999999999993</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="2"/>
+        <v>23.051538461538399</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="3"/>
+        <v>23.369372976941364</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="4"/>
+        <v>0.72778060390247523</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>5</v>
       </c>
@@ -914,8 +1728,34 @@
       <c r="D32">
         <v>0.10070999999999999</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E32">
+        <v>1.2250300000000001</v>
+      </c>
+      <c r="F32" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="0"/>
+        <v>4.083153846153853E-2</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="1"/>
+        <v>547.1</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="2"/>
+        <v>40.831538461538528</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="3"/>
+        <v>13.398956312051371</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="4"/>
+        <v>0.59456321654713007</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>5</v>
       </c>
@@ -928,8 +1768,34 @@
       <c r="D33">
         <v>5.5039999999999999E-2</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E33">
+        <v>1.21045</v>
+      </c>
+      <c r="F33" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="0"/>
+        <v>2.6251538461538493E-2</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="1"/>
+        <v>371.6</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="2"/>
+        <v>26.251538461538495</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="3"/>
+        <v>14.155360857971678</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="4"/>
+        <v>0.52304617620751281</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>5</v>
       </c>
@@ -942,8 +1808,34 @@
       <c r="D34">
         <v>6.9680000000000006E-2</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E34">
+        <v>1.1863300000000001</v>
+      </c>
+      <c r="F34">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="0"/>
+        <v>2.1315384615385735E-3</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="1"/>
+        <v>388.7</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="2"/>
+        <v>2.1315384615385735</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="3"/>
+        <v>182.35654998194639</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="4"/>
+        <v>0.96940960876092752</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>5</v>
       </c>
@@ -956,8 +1848,34 @@
       <c r="D35">
         <v>9.6759999999999999E-2</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E35">
+        <v>1.2108699999999999</v>
+      </c>
+      <c r="F35" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="0"/>
+        <v>2.6671538461538358E-2</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="1"/>
+        <v>755.6</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="2"/>
+        <v>26.671538461538358</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="3"/>
+        <v>28.329824359011447</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="4"/>
+        <v>0.72435367443635434</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>5</v>
       </c>
@@ -970,8 +1888,34 @@
       <c r="D36">
         <v>0.17977000000000001</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E36">
+        <v>1.22305</v>
+      </c>
+      <c r="F36" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="0"/>
+        <v>3.8851538461538437E-2</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="1"/>
+        <v>905.00000000000011</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="2"/>
+        <v>38.851538461538439</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="3"/>
+        <v>23.293800859286847</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="4"/>
+        <v>0.78388196884052719</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>5</v>
       </c>
@@ -984,8 +1928,34 @@
       <c r="D37">
         <v>4.8570000000000002E-2</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E37">
+        <v>1.2066600000000001</v>
+      </c>
+      <c r="F37" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="0"/>
+        <v>2.2461538461538533E-2</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="1"/>
+        <v>342.8</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="2"/>
+        <v>22.461538461538531</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="3"/>
+        <v>15.261643835616391</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="4"/>
+        <v>0.53754295940830699</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>5</v>
       </c>
@@ -998,8 +1968,34 @@
       <c r="D38">
         <v>3.8969999999999998E-2</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E38">
+        <v>1.1900900000000001</v>
+      </c>
+      <c r="F38" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="0"/>
+        <v>5.8915384615385591E-3</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="1"/>
+        <v>218.7</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="2"/>
+        <v>5.8915384615385591</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="3"/>
+        <v>37.121034077555201</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="4"/>
+        <v>0.84881861787173318</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>5</v>
       </c>
@@ -1012,8 +2008,34 @@
       <c r="D39">
         <v>6.4460000000000003E-2</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E39">
+        <v>1.2136400000000001</v>
+      </c>
+      <c r="F39" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="0"/>
+        <v>2.9441538461538519E-2</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="1"/>
+        <v>369.09999999999997</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="2"/>
+        <v>29.441538461538521</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="3"/>
+        <v>12.536708993050086</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="4"/>
+        <v>0.54325878899257651</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>5</v>
       </c>
@@ -1026,8 +2048,34 @@
       <c r="D40">
         <v>9.8280000000000006E-2</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E40">
+        <v>1.18797</v>
+      </c>
+      <c r="F40">
+        <v>1.16916</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="0"/>
+        <v>1.8809999999999993E-2</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="1"/>
+        <v>529.69999999999993</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="2"/>
+        <v>18.809999999999995</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="3"/>
+        <v>28.160552897395007</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="4"/>
+        <v>0.80860805860805873</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>5</v>
       </c>
@@ -1040,8 +2088,34 @@
       <c r="D41">
         <v>5.0930000000000003E-2</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E41">
+        <v>1.18919</v>
+      </c>
+      <c r="F41">
+        <v>1.1817800000000001</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="0"/>
+        <v>7.4099999999999167E-3</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="1"/>
+        <v>268.40000000000003</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="2"/>
+        <v>7.4099999999999167</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="3"/>
+        <v>36.221322537112421</v>
+      </c>
+      <c r="K41">
+        <f t="shared" si="4"/>
+        <v>0.85450618495975028</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>6</v>
       </c>
@@ -1054,8 +2128,34 @@
       <c r="D42">
         <v>0.24798999999999999</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E42">
+        <v>1.3030200000000001</v>
+      </c>
+      <c r="F42" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="0"/>
+        <v>0.11882153846153853</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="1"/>
+        <v>1037.4000000000001</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="2"/>
+        <v>118.82153846153854</v>
+      </c>
+      <c r="J42">
+        <f t="shared" si="3"/>
+        <v>8.7307403475153382</v>
+      </c>
+      <c r="K42">
+        <f t="shared" si="4"/>
+        <v>0.52086157320239312</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>6</v>
       </c>
@@ -1068,8 +2168,34 @@
       <c r="D43">
         <v>0.12002</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E43">
+        <v>1.2276199999999999</v>
+      </c>
+      <c r="F43" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="0"/>
+        <v>4.34215384615384E-2</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="1"/>
+        <v>522.20000000000005</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="2"/>
+        <v>43.421538461538404</v>
+      </c>
+      <c r="J43">
+        <f t="shared" si="3"/>
+        <v>12.0262896825397</v>
+      </c>
+      <c r="K43">
+        <f t="shared" si="4"/>
+        <v>0.63821414379654728</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>6</v>
       </c>
@@ -1082,8 +2208,34 @@
       <c r="D44">
         <v>0.12544</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E44">
+        <v>1.2495000000000001</v>
+      </c>
+      <c r="F44" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="0"/>
+        <v>6.5301538461538522E-2</v>
+      </c>
+      <c r="H44">
+        <f t="shared" si="1"/>
+        <v>617.79999999999995</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="2"/>
+        <v>65.301538461538527</v>
+      </c>
+      <c r="J44">
+        <f t="shared" si="3"/>
+        <v>9.4607265702304009</v>
+      </c>
+      <c r="K44">
+        <f t="shared" si="4"/>
+        <v>0.47942013343799006</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>6</v>
       </c>
@@ -1096,8 +2248,34 @@
       <c r="D45">
         <v>0.18249000000000001</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E45">
+        <v>1.26292</v>
+      </c>
+      <c r="F45" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="0"/>
+        <v>7.8721538461538509E-2</v>
+      </c>
+      <c r="H45">
+        <f t="shared" si="1"/>
+        <v>1104.5</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="2"/>
+        <v>78.721538461538515</v>
+      </c>
+      <c r="J45">
+        <f t="shared" si="3"/>
+        <v>14.030467665969621</v>
+      </c>
+      <c r="K45">
+        <f t="shared" si="4"/>
+        <v>0.56862546735964437</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>6</v>
       </c>
@@ -1110,8 +2288,34 @@
       <c r="D46">
         <v>0.1168</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E46">
+        <v>1.2212400000000001</v>
+      </c>
+      <c r="F46" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="0"/>
+        <v>3.704153846153857E-2</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="1"/>
+        <v>579</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="2"/>
+        <v>37.041538461538572</v>
+      </c>
+      <c r="J46">
+        <f t="shared" si="3"/>
+        <v>15.631100220127045</v>
+      </c>
+      <c r="K46">
+        <f t="shared" si="4"/>
+        <v>0.6828635405690191</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>6</v>
       </c>
@@ -1124,8 +2328,34 @@
       <c r="D47">
         <v>7.9450000000000007E-2</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E47">
+        <v>1.19411</v>
+      </c>
+      <c r="F47" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="0"/>
+        <v>9.9115384615384716E-3</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="1"/>
+        <v>468.29999999999995</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="2"/>
+        <v>9.9115384615384716</v>
+      </c>
+      <c r="J47">
+        <f t="shared" si="3"/>
+        <v>47.247962747380626</v>
+      </c>
+      <c r="K47">
+        <f t="shared" si="4"/>
+        <v>0.87524809991770336</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>6</v>
       </c>
@@ -1138,8 +2368,34 @@
       <c r="D48">
         <v>0.16702</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E48">
+        <v>1.24072</v>
+      </c>
+      <c r="F48" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G48">
+        <f t="shared" si="0"/>
+        <v>5.6521538461538512E-2</v>
+      </c>
+      <c r="H48">
+        <f t="shared" si="1"/>
+        <v>853.40000000000009</v>
+      </c>
+      <c r="I48">
+        <f t="shared" si="2"/>
+        <v>56.521538461538512</v>
+      </c>
+      <c r="J48">
+        <f t="shared" si="3"/>
+        <v>15.098668989357346</v>
+      </c>
+      <c r="K48">
+        <f t="shared" si="4"/>
+        <v>0.66158820224201587</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>6</v>
       </c>
@@ -1152,8 +2408,34 @@
       <c r="D49">
         <v>0.17754</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E49">
+        <v>1.2929900000000001</v>
+      </c>
+      <c r="F49" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G49">
+        <f t="shared" si="0"/>
+        <v>0.10879153846153855</v>
+      </c>
+      <c r="H49">
+        <f t="shared" si="1"/>
+        <v>941</v>
+      </c>
+      <c r="I49">
+        <f t="shared" si="2"/>
+        <v>108.79153846153855</v>
+      </c>
+      <c r="J49">
+        <f t="shared" si="3"/>
+        <v>8.6495697487785321</v>
+      </c>
+      <c r="K49">
+        <f t="shared" si="4"/>
+        <v>0.38722801362206516</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>6</v>
       </c>
@@ -1166,8 +2448,34 @@
       <c r="D50">
         <v>0.17058999999999999</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E50">
+        <v>1.2536400000000001</v>
+      </c>
+      <c r="F50" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G50">
+        <f t="shared" si="0"/>
+        <v>6.9441538461538554E-2</v>
+      </c>
+      <c r="H50">
+        <f t="shared" si="1"/>
+        <v>762.8</v>
+      </c>
+      <c r="I50">
+        <f t="shared" si="2"/>
+        <v>69.441538461538556</v>
+      </c>
+      <c r="J50">
+        <f t="shared" si="3"/>
+        <v>10.984779670780053</v>
+      </c>
+      <c r="K50">
+        <f t="shared" si="4"/>
+        <v>0.59293312350349636</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>6</v>
       </c>
@@ -1180,8 +2488,34 @@
       <c r="D51">
         <v>8.158E-2</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E51">
+        <v>1.2329000000000001</v>
+      </c>
+      <c r="F51" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="0"/>
+        <v>4.8701538461538574E-2</v>
+      </c>
+      <c r="H51">
+        <f t="shared" si="1"/>
+        <v>437.8</v>
+      </c>
+      <c r="I51">
+        <f t="shared" si="2"/>
+        <v>48.701538461538576</v>
+      </c>
+      <c r="J51">
+        <f t="shared" si="3"/>
+        <v>8.9894490775840072</v>
+      </c>
+      <c r="K51">
+        <f t="shared" si="4"/>
+        <v>0.40302110245723738</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>6</v>
       </c>
@@ -1194,8 +2528,34 @@
       <c r="D52">
         <v>0.14607000000000001</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E52">
+        <v>1.2270399999999999</v>
+      </c>
+      <c r="F52" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G52">
+        <f t="shared" si="0"/>
+        <v>4.2841538461538375E-2</v>
+      </c>
+      <c r="H52">
+        <f t="shared" si="1"/>
+        <v>719.80000000000007</v>
+      </c>
+      <c r="I52">
+        <f t="shared" si="2"/>
+        <v>42.841538461538377</v>
+      </c>
+      <c r="J52">
+        <f t="shared" si="3"/>
+        <v>16.8014507846447</v>
+      </c>
+      <c r="K52">
+        <f t="shared" si="4"/>
+        <v>0.70670542574424333</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>6</v>
       </c>
@@ -1208,8 +2568,34 @@
       <c r="D53">
         <v>0.18551000000000001</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E53">
+        <v>1.2575700000000001</v>
+      </c>
+      <c r="F53" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G53">
+        <f t="shared" si="0"/>
+        <v>7.3371538461538544E-2</v>
+      </c>
+      <c r="H53">
+        <f t="shared" si="1"/>
+        <v>955.19999999999993</v>
+      </c>
+      <c r="I53">
+        <f t="shared" si="2"/>
+        <v>73.371538461538549</v>
+      </c>
+      <c r="J53">
+        <f t="shared" si="3"/>
+        <v>13.018672090414418</v>
+      </c>
+      <c r="K53">
+        <f t="shared" si="4"/>
+        <v>0.60448742137060785</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>6</v>
       </c>
@@ -1222,8 +2608,34 @@
       <c r="D54">
         <v>0.15151999999999999</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E54">
+        <v>1.2661500000000001</v>
+      </c>
+      <c r="F54" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G54">
+        <f t="shared" si="0"/>
+        <v>8.1951538461538576E-2</v>
+      </c>
+      <c r="H54">
+        <f t="shared" si="1"/>
+        <v>682.80000000000007</v>
+      </c>
+      <c r="I54">
+        <f t="shared" si="2"/>
+        <v>81.951538461538576</v>
+      </c>
+      <c r="J54">
+        <f t="shared" si="3"/>
+        <v>8.3317532875902156</v>
+      </c>
+      <c r="K54">
+        <f t="shared" si="4"/>
+        <v>0.45913715376492487</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>6</v>
       </c>
@@ -1236,8 +2648,34 @@
       <c r="D55">
         <v>0.22428000000000001</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E55">
+        <v>1.2569999999999999</v>
+      </c>
+      <c r="F55" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G55">
+        <f t="shared" si="0"/>
+        <v>7.2801538461538362E-2</v>
+      </c>
+      <c r="H55">
+        <f t="shared" si="1"/>
+        <v>1148.6000000000001</v>
+      </c>
+      <c r="I55">
+        <f t="shared" si="2"/>
+        <v>72.801538461538357</v>
+      </c>
+      <c r="J55">
+        <f t="shared" si="3"/>
+        <v>15.777139113712753</v>
+      </c>
+      <c r="K55">
+        <f t="shared" si="4"/>
+        <v>0.67539888326405229</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>6</v>
       </c>
@@ -1250,8 +2688,34 @@
       <c r="D56">
         <v>0.13436999999999999</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E56">
+        <v>1.2558</v>
+      </c>
+      <c r="F56" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G56">
+        <f t="shared" si="0"/>
+        <v>7.1601538461538494E-2</v>
+      </c>
+      <c r="H56">
+        <f t="shared" si="1"/>
+        <v>722.8</v>
+      </c>
+      <c r="I56">
+        <f t="shared" si="2"/>
+        <v>71.601538461538496</v>
+      </c>
+      <c r="J56">
+        <f t="shared" si="3"/>
+        <v>10.094755162115119</v>
+      </c>
+      <c r="K56">
+        <f t="shared" si="4"/>
+        <v>0.46713151401697922</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>6</v>
       </c>
@@ -1264,8 +2728,34 @@
       <c r="D57">
         <v>0.13617000000000001</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E57">
+        <v>1.25908</v>
+      </c>
+      <c r="F57" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G57">
+        <f t="shared" si="0"/>
+        <v>7.4881538461538444E-2</v>
+      </c>
+      <c r="H57">
+        <f t="shared" si="1"/>
+        <v>746.5</v>
+      </c>
+      <c r="I57">
+        <f t="shared" si="2"/>
+        <v>74.88153846153844</v>
+      </c>
+      <c r="J57">
+        <f t="shared" si="3"/>
+        <v>9.9690793663838289</v>
+      </c>
+      <c r="K57">
+        <f t="shared" si="4"/>
+        <v>0.45008784268533131</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>6</v>
       </c>
@@ -1278,8 +2768,34 @@
       <c r="D58">
         <v>0.25195000000000001</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E58">
+        <v>1.2695099999999999</v>
+      </c>
+      <c r="F58" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G58">
+        <f t="shared" si="0"/>
+        <v>8.5311538461538383E-2</v>
+      </c>
+      <c r="H58">
+        <f t="shared" si="1"/>
+        <v>1571.3</v>
+      </c>
+      <c r="I58">
+        <f t="shared" si="2"/>
+        <v>85.31153846153839</v>
+      </c>
+      <c r="J58">
+        <f t="shared" si="3"/>
+        <v>18.418376087642592</v>
+      </c>
+      <c r="K58">
+        <f t="shared" si="4"/>
+        <v>0.66139496542354281</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>6</v>
       </c>
@@ -1292,8 +2808,34 @@
       <c r="D59">
         <v>0.21695999999999999</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E59">
+        <v>1.3063800000000001</v>
+      </c>
+      <c r="F59" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G59">
+        <f t="shared" si="0"/>
+        <v>0.12218153846153856</v>
+      </c>
+      <c r="H59">
+        <f t="shared" si="1"/>
+        <v>1084.3</v>
+      </c>
+      <c r="I59">
+        <f t="shared" si="2"/>
+        <v>122.18153846153857</v>
+      </c>
+      <c r="J59">
+        <f t="shared" si="3"/>
+        <v>8.8744994837442306</v>
+      </c>
+      <c r="K59">
+        <f t="shared" si="4"/>
+        <v>0.43684762877240702</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>6</v>
       </c>
@@ -1306,8 +2848,34 @@
       <c r="D60">
         <v>0.22137999999999999</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E60">
+        <v>1.25299</v>
+      </c>
+      <c r="F60" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G60">
+        <f t="shared" si="0"/>
+        <v>6.8791538461538515E-2</v>
+      </c>
+      <c r="H60">
+        <f t="shared" si="1"/>
+        <v>1143</v>
+      </c>
+      <c r="I60">
+        <f t="shared" si="2"/>
+        <v>68.791538461538522</v>
+      </c>
+      <c r="J60">
+        <f t="shared" si="3"/>
+        <v>16.615415581075474</v>
+      </c>
+      <c r="K60">
+        <f t="shared" si="4"/>
+        <v>0.68926037373954951</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>6</v>
       </c>
@@ -1320,8 +2888,34 @@
       <c r="D61">
         <v>0.24229000000000001</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E61">
+        <v>1.28416</v>
+      </c>
+      <c r="F61" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G61">
+        <f t="shared" si="0"/>
+        <v>9.9961538461538435E-2</v>
+      </c>
+      <c r="H61">
+        <f t="shared" si="1"/>
+        <v>1566.6000000000001</v>
+      </c>
+      <c r="I61">
+        <f t="shared" si="2"/>
+        <v>99.961538461538439</v>
+      </c>
+      <c r="J61">
+        <f t="shared" si="3"/>
+        <v>15.672027702962684</v>
+      </c>
+      <c r="K61">
+        <f t="shared" si="4"/>
+        <v>0.58743019331570256</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>3</v>
       </c>
@@ -1334,8 +2928,33 @@
       <c r="D62">
         <v>0.33822000000000002</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E62">
+        <v>1.35171</v>
+      </c>
+      <c r="F62" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G62">
+        <f t="shared" si="0"/>
+        <v>0.16751153846153843</v>
+      </c>
+      <c r="H62" t="s">
+        <v>9</v>
+      </c>
+      <c r="I62">
+        <f t="shared" si="2"/>
+        <v>167.51153846153844</v>
+      </c>
+      <c r="J62" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K62">
+        <f t="shared" si="4"/>
+        <v>0.5047260999895381</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>3</v>
       </c>
@@ -1348,8 +2967,33 @@
       <c r="D63">
         <v>0.24389</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E63">
+        <v>1.3071699999999999</v>
+      </c>
+      <c r="F63" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G63">
+        <f t="shared" si="0"/>
+        <v>0.12297153846153841</v>
+      </c>
+      <c r="H63" t="s">
+        <v>9</v>
+      </c>
+      <c r="I63">
+        <f t="shared" si="2"/>
+        <v>122.97153846153842</v>
+      </c>
+      <c r="J63" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K63">
+        <f t="shared" si="4"/>
+        <v>0.49579097764755253</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>3</v>
       </c>
@@ -1362,8 +3006,33 @@
       <c r="D64">
         <v>0.22101000000000001</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E64">
+        <v>1.2988999999999999</v>
+      </c>
+      <c r="F64" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G64">
+        <f t="shared" si="0"/>
+        <v>0.11470153846153841</v>
+      </c>
+      <c r="H64" t="s">
+        <v>9</v>
+      </c>
+      <c r="I64">
+        <f t="shared" si="2"/>
+        <v>114.70153846153841</v>
+      </c>
+      <c r="J64" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K64">
+        <f t="shared" si="4"/>
+        <v>0.48101199736872358</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>3</v>
       </c>
@@ -1376,8 +3045,33 @@
       <c r="D65">
         <v>0.47436</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E65">
+        <v>1.4298200000000001</v>
+      </c>
+      <c r="F65" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G65">
+        <f t="shared" si="0"/>
+        <v>0.24562153846153856</v>
+      </c>
+      <c r="H65" t="s">
+        <v>9</v>
+      </c>
+      <c r="I65">
+        <f t="shared" si="2"/>
+        <v>245.62153846153856</v>
+      </c>
+      <c r="J65" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K65">
+        <f t="shared" si="4"/>
+        <v>0.48220436280137752</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>3</v>
       </c>
@@ -1390,8 +3084,33 @@
       <c r="D66">
         <v>0.29764000000000002</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E66">
+        <v>1.32833</v>
+      </c>
+      <c r="F66" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G66">
+        <f t="shared" si="0"/>
+        <v>0.14413153846153848</v>
+      </c>
+      <c r="H66" t="s">
+        <v>9</v>
+      </c>
+      <c r="I66">
+        <f t="shared" si="2"/>
+        <v>144.13153846153847</v>
+      </c>
+      <c r="J66" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K66">
+        <f t="shared" si="4"/>
+        <v>0.51575212181985464</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>3</v>
       </c>
@@ -1404,8 +3123,33 @@
       <c r="D67">
         <v>0.14144000000000001</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E67">
+        <v>1.2457800000000001</v>
+      </c>
+      <c r="F67" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G67">
+        <f t="shared" ref="G67:G81" si="5">E67-F67</f>
+        <v>6.1581538461538576E-2</v>
+      </c>
+      <c r="H67" t="s">
+        <v>9</v>
+      </c>
+      <c r="I67">
+        <f t="shared" ref="I67:I81" si="6">G67*1000</f>
+        <v>61.581538461538578</v>
+      </c>
+      <c r="J67" t="e">
+        <f t="shared" ref="J67:J81" si="7">H67/I67</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K67">
+        <f t="shared" ref="K67:K81" si="8">(D67-G67)/D67</f>
+        <v>0.56461016359206329</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>3</v>
       </c>
@@ -1418,8 +3162,33 @@
       <c r="D68">
         <v>0.23454</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E68">
+        <v>1.32334</v>
+      </c>
+      <c r="F68" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G68">
+        <f t="shared" si="5"/>
+        <v>0.13914153846153843</v>
+      </c>
+      <c r="H68" t="s">
+        <v>9</v>
+      </c>
+      <c r="I68">
+        <f t="shared" si="6"/>
+        <v>139.14153846153843</v>
+      </c>
+      <c r="J68" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K68">
+        <f t="shared" si="8"/>
+        <v>0.406747085948928</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>3</v>
       </c>
@@ -1432,8 +3201,33 @@
       <c r="D69">
         <v>0.18940000000000001</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E69">
+        <v>1.2972399999999999</v>
+      </c>
+      <c r="F69" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G69">
+        <f t="shared" si="5"/>
+        <v>0.11304153846153842</v>
+      </c>
+      <c r="H69" t="s">
+        <v>9</v>
+      </c>
+      <c r="I69">
+        <f t="shared" si="6"/>
+        <v>113.04153846153841</v>
+      </c>
+      <c r="J69" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K69">
+        <f t="shared" si="8"/>
+        <v>0.40315977581025125</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>3</v>
       </c>
@@ -1446,8 +3240,33 @@
       <c r="D70">
         <v>0.23415</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E70">
+        <v>1.2977700000000001</v>
+      </c>
+      <c r="F70" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G70">
+        <f t="shared" si="5"/>
+        <v>0.11357153846153856</v>
+      </c>
+      <c r="H70" t="s">
+        <v>9</v>
+      </c>
+      <c r="I70">
+        <f t="shared" si="6"/>
+        <v>113.57153846153855</v>
+      </c>
+      <c r="J70" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K70">
+        <f t="shared" si="8"/>
+        <v>0.51496246653197286</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>3</v>
       </c>
@@ -1460,8 +3279,33 @@
       <c r="D71">
         <v>0.38391999999999998</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E71">
+        <v>1.3834900000000001</v>
+      </c>
+      <c r="F71" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G71">
+        <f t="shared" si="5"/>
+        <v>0.19929153846153858</v>
+      </c>
+      <c r="H71" t="s">
+        <v>9</v>
+      </c>
+      <c r="I71">
+        <f t="shared" si="6"/>
+        <v>199.29153846153858</v>
+      </c>
+      <c r="J71" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K71">
+        <f t="shared" si="8"/>
+        <v>0.48090347348005164</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>3</v>
       </c>
@@ -1474,8 +3318,33 @@
       <c r="D72">
         <v>0.57989000000000002</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E72">
+        <v>1.51153</v>
+      </c>
+      <c r="F72" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G72">
+        <f t="shared" si="5"/>
+        <v>0.32733153846153851</v>
+      </c>
+      <c r="H72" t="s">
+        <v>9</v>
+      </c>
+      <c r="I72">
+        <f t="shared" si="6"/>
+        <v>327.33153846153851</v>
+      </c>
+      <c r="J72" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K72">
+        <f t="shared" si="8"/>
+        <v>0.43552822352249826</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>3</v>
       </c>
@@ -1488,8 +3357,33 @@
       <c r="D73">
         <v>0.12059</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E73">
+        <v>1.2694399999999999</v>
+      </c>
+      <c r="F73" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G73">
+        <f t="shared" si="5"/>
+        <v>8.5241538461538369E-2</v>
+      </c>
+      <c r="H73" t="s">
+        <v>9</v>
+      </c>
+      <c r="I73">
+        <f t="shared" si="6"/>
+        <v>85.241538461538369</v>
+      </c>
+      <c r="J73" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K73">
+        <f t="shared" si="8"/>
+        <v>0.29312929379269953</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>3</v>
       </c>
@@ -1502,8 +3396,33 @@
       <c r="D74">
         <v>0.51493</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E74">
+        <v>1.4576899999999999</v>
+      </c>
+      <c r="F74" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G74">
+        <f t="shared" si="5"/>
+        <v>0.2734915384615384</v>
+      </c>
+      <c r="H74" t="s">
+        <v>9</v>
+      </c>
+      <c r="I74">
+        <f t="shared" si="6"/>
+        <v>273.49153846153843</v>
+      </c>
+      <c r="J74" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K74">
+        <f t="shared" si="8"/>
+        <v>0.46887627743278038</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>3</v>
       </c>
@@ -1516,8 +3435,33 @@
       <c r="D75">
         <v>0.39989999999999998</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E75">
+        <v>1.4584299999999999</v>
+      </c>
+      <c r="F75" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G75">
+        <f t="shared" si="5"/>
+        <v>0.27423153846153836</v>
+      </c>
+      <c r="H75" t="s">
+        <v>9</v>
+      </c>
+      <c r="I75">
+        <f t="shared" si="6"/>
+        <v>274.23153846153838</v>
+      </c>
+      <c r="J75" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K75">
+        <f t="shared" si="8"/>
+        <v>0.31424971627522286</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>3</v>
       </c>
@@ -1530,8 +3474,33 @@
       <c r="D76">
         <v>0.4587</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E76">
+        <v>1.40405</v>
+      </c>
+      <c r="F76" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G76">
+        <f t="shared" si="5"/>
+        <v>0.21985153846153849</v>
+      </c>
+      <c r="H76" t="s">
+        <v>9</v>
+      </c>
+      <c r="I76">
+        <f t="shared" si="6"/>
+        <v>219.8515384615385</v>
+      </c>
+      <c r="J76" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K76">
+        <f t="shared" si="8"/>
+        <v>0.52070735020375303</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>3</v>
       </c>
@@ -1544,8 +3513,33 @@
       <c r="D77">
         <v>0.47954999999999998</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E77">
+        <v>1.45329</v>
+      </c>
+      <c r="F77" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G77">
+        <f t="shared" si="5"/>
+        <v>0.26909153846153844</v>
+      </c>
+      <c r="H77" t="s">
+        <v>9</v>
+      </c>
+      <c r="I77">
+        <f t="shared" si="6"/>
+        <v>269.09153846153845</v>
+      </c>
+      <c r="J77" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K77">
+        <f t="shared" si="8"/>
+        <v>0.43886656561038795</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>3</v>
       </c>
@@ -1558,8 +3552,33 @@
       <c r="D78">
         <v>0.2177</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E78">
+        <v>1.2943800000000001</v>
+      </c>
+      <c r="F78" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G78">
+        <f t="shared" si="5"/>
+        <v>0.11018153846153855</v>
+      </c>
+      <c r="H78" t="s">
+        <v>9</v>
+      </c>
+      <c r="I78">
+        <f t="shared" si="6"/>
+        <v>110.18153846153855</v>
+      </c>
+      <c r="J78" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K78">
+        <f t="shared" si="8"/>
+        <v>0.49388360835306133</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>3</v>
       </c>
@@ -1572,8 +3591,33 @@
       <c r="D79">
         <v>0.18076</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E79">
+        <v>1.2820400000000001</v>
+      </c>
+      <c r="F79" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G79">
+        <f t="shared" si="5"/>
+        <v>9.7841538461538535E-2</v>
+      </c>
+      <c r="H79" t="s">
+        <v>9</v>
+      </c>
+      <c r="I79">
+        <f t="shared" si="6"/>
+        <v>97.841538461538534</v>
+      </c>
+      <c r="J79" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K79">
+        <f t="shared" si="8"/>
+        <v>0.45872129640662462</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>3</v>
       </c>
@@ -1586,8 +3630,33 @@
       <c r="D80">
         <v>0.37152000000000002</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E80">
+        <v>1.39398</v>
+      </c>
+      <c r="F80" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G80">
+        <f t="shared" si="5"/>
+        <v>0.20978153846153846</v>
+      </c>
+      <c r="H80" t="s">
+        <v>9</v>
+      </c>
+      <c r="I80">
+        <f t="shared" si="6"/>
+        <v>209.78153846153847</v>
+      </c>
+      <c r="J80" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K80">
+        <f t="shared" si="8"/>
+        <v>0.43534254290068247</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>3</v>
       </c>
@@ -1599,6 +3668,31 @@
       </c>
       <c r="D81">
         <v>0.42020000000000002</v>
+      </c>
+      <c r="E81">
+        <v>1.40188</v>
+      </c>
+      <c r="F81" s="1">
+        <v>1.1841984615384615</v>
+      </c>
+      <c r="G81">
+        <f t="shared" si="5"/>
+        <v>0.21768153846153848</v>
+      </c>
+      <c r="H81" t="s">
+        <v>9</v>
+      </c>
+      <c r="I81">
+        <f t="shared" si="6"/>
+        <v>217.68153846153848</v>
+      </c>
+      <c r="J81" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K81">
+        <f t="shared" si="8"/>
+        <v>0.48195730970600076</v>
       </c>
     </row>
   </sheetData>

</xml_diff>